<commit_message>
Added UI in UI.xlsx and edited css
Signed-off-by: Rohan <rohan9969@gmail.com>
</commit_message>
<xml_diff>
--- a/Gila_Breath_Camp/Documents/UI.xlsx
+++ b/Gila_Breath_Camp/Documents/UI.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17426"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9735" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9735" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="LoginScreen" sheetId="1" r:id="rId1"/>
@@ -16,13 +16,14 @@
     <sheet name="CheckIn" sheetId="7" r:id="rId7"/>
     <sheet name="Separate Questions" sheetId="8" r:id="rId8"/>
     <sheet name="CustomerPriorities" sheetId="10" r:id="rId9"/>
+    <sheet name="Sheet2" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
   <si>
     <t>The purpose to add this screen:</t>
   </si>
@@ -165,6 +166,34 @@
   </si>
   <si>
     <t>virtual thing which actuallly doesn’t need coding</t>
+  </si>
+  <si>
+    <t>Appl No</t>
+  </si>
+  <si>
+    <t>Applicant Name</t>
+  </si>
+  <si>
+    <t>Applicant Name 
+(Together with)</t>
+  </si>
+  <si>
+    <t>Guardian SSN
+ (Together with)</t>
+  </si>
+  <si>
+    <t>Applicant Name 
+(Not Together with)</t>
+  </si>
+  <si>
+    <t>Guardian SSN 
+(Not Together with)</t>
+  </si>
+  <si>
+    <t>Gohil, Jemin</t>
+  </si>
+  <si>
+    <t>Manjunath, Karthik</t>
   </si>
 </sst>
 </file>
@@ -460,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -496,6 +525,9 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6457,6 +6489,66 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="7" width="18.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A16:A17"/>
@@ -6918,7 +7010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A20:O29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="V9" sqref="L1:V9"/>
     </sheetView>
   </sheetViews>

</xml_diff>